<commit_message>
excel changes for timestamp
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NTVNSV31\Documents\selenium\cucumber java\Load-test\src\test\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16020" windowHeight="6030" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16020" windowHeight="6345" tabRatio="721" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestCaseRun" sheetId="2" r:id="rId1"/>
@@ -21,6 +16,7 @@
     <sheet name="TC005" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:G19"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="29">
   <si>
     <t>www20.thegeneraltest.com/news/</t>
   </si>
@@ -108,6 +104,15 @@
   </si>
   <si>
     <t>https://www20.thegeneraltest.com/quote/</t>
+  </si>
+  <si>
+    <t>Time of Execution</t>
+  </si>
+  <si>
+    <t>2019/05/21 15:30:10</t>
+  </si>
+  <si>
+    <t>2019/05/21 15:45:36</t>
   </si>
 </sst>
 </file>
@@ -996,19 +1001,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="40" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1018,8 +1025,11 @@
       <c r="C1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>31.52</v>
       </c>
@@ -1030,7 +1040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>31.385000000000002</v>
       </c>
@@ -1039,6 +1049,62 @@
       </c>
       <c r="C3">
         <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>31.073</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>31.446999999999999</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>31.303999999999998</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>31.47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1048,20 +1114,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1071,8 +1138,11 @@
       <c r="C1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>31.739000000000001</v>
       </c>
@@ -1083,7 +1153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>31.635000000000002</v>
       </c>
@@ -1092,6 +1162,62 @@
       </c>
       <c r="C3">
         <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>32.154000000000003</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>31.373000000000001</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>31.847999999999999</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>32.621000000000002</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1101,15 +1227,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="41.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="33.42578125" customWidth="1" collapsed="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1118,6 +1250,9 @@
       </c>
       <c r="C1" t="s">
         <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1127,15 +1262,21 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="53" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1144,6 +1285,9 @@
       </c>
       <c r="C1" t="s">
         <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1153,15 +1297,21 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1" collapsed="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1170,6 +1320,9 @@
       </c>
       <c r="C1" t="s">
         <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>